<commit_message>
Update test results with changes from residue and crop coefficient changes
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS1/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS1/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11870EA-8596-4D90-B2A0-EBF62CD03823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A669FA1-A15A-44C1-B9BA-B374C435E70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="LincolnRot1" sheetId="3" r:id="rId1"/>
@@ -419,9 +419,6 @@
     <t>LincolnRot2_N1_Irr2_RyeGrass</t>
   </si>
   <si>
-    <t>Hastings</t>
-  </si>
-  <si>
     <t>Clay loam</t>
   </si>
   <si>
@@ -477,6 +474,9 @@
   </si>
   <si>
     <t>Very Wet</t>
+  </si>
+  <si>
+    <t>hastings</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A90A1-2F9B-4EC2-8DA6-AD1920316E14}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
@@ -1855,7 +1855,7 @@
         <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" t="s">
         <v>80</v>
@@ -1867,7 +1867,7 @@
         <v>57</v>
       </c>
       <c r="J24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K24" s="12"/>
     </row>
@@ -2180,7 +2180,7 @@
         <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -2192,7 +2192,7 @@
         <v>57</v>
       </c>
       <c r="I35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>70</v>
@@ -3317,7 +3317,7 @@
         <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" t="s">
         <v>91</v>
@@ -3329,7 +3329,7 @@
         <v>95</v>
       </c>
       <c r="J24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -3658,7 +3658,7 @@
         <v>95</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -3670,7 +3670,7 @@
         <v>95</v>
       </c>
       <c r="I35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>70</v>
@@ -4111,8 +4111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AD42EA-A0EE-4986-A449-DEBA14E52DE4}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4132,16 +4132,16 @@
         <v>55</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>106</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>107</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -4162,16 +4162,16 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -4216,16 +4216,16 @@
         <v>73</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -4575,13 +4575,13 @@
         <v>57</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -4793,13 +4793,13 @@
         <v>36</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>70</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -5104,8 +5104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B8B917-5635-4965-8A45-89E9AEAAEA05}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5127,34 +5127,34 @@
         <v>55</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>110</v>
-      </c>
       <c r="F1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>118</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>119</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
@@ -5170,34 +5170,34 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="K2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="L2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -5278,34 +5278,34 @@
         <v>73</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -5506,7 +5506,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>6</v>
@@ -5521,7 +5521,7 @@
         <v>6</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5579,10 +5579,10 @@
         <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>59</v>
@@ -5594,10 +5594,10 @@
         <v>91</v>
       </c>
       <c r="J13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>59</v>
@@ -5974,31 +5974,31 @@
         <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>91</v>
       </c>
       <c r="I24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>59</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
@@ -6379,31 +6379,31 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>59</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G35" s="31" t="s">
         <v>70</v>
       </c>
       <c r="H35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J35" s="16" t="s">
         <v>59</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L35" s="31" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
getting WS1 graphs working
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS1/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS1/FieldConfigs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A669FA1-A15A-44C1-B9BA-B374C435E70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544B4564-2438-4D44-B766-8B313093D0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
@@ -422,18 +422,6 @@
     <t>Clay loam</t>
   </si>
   <si>
-    <t>HawkesBayRot3_N1_irr1_Onion</t>
-  </si>
-  <si>
-    <t>HawkesBayRot3_N1_irr1_Ryegrass</t>
-  </si>
-  <si>
-    <t>HawkesBayRot3_N1_irr2_Onion</t>
-  </si>
-  <si>
-    <t>HawkesBayRot3_N1_irr2_Ryegrass</t>
-  </si>
-  <si>
     <t>Lettuce Vegetable Ice berg</t>
   </si>
   <si>
@@ -477,6 +465,18 @@
   </si>
   <si>
     <t>hastings</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr1_Onion</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr1_Ryegrass</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr2_Onion</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr2_Ryegrass</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1855,7 @@
         <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G24" t="s">
         <v>80</v>
@@ -1867,7 +1867,7 @@
         <v>57</v>
       </c>
       <c r="J24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K24" s="12"/>
     </row>
@@ -2180,7 +2180,7 @@
         <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -2192,7 +2192,7 @@
         <v>57</v>
       </c>
       <c r="I35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>70</v>
@@ -3317,7 +3317,7 @@
         <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G24" t="s">
         <v>91</v>
@@ -3329,7 +3329,7 @@
         <v>95</v>
       </c>
       <c r="J24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -3658,7 +3658,7 @@
         <v>95</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -3670,7 +3670,7 @@
         <v>95</v>
       </c>
       <c r="I35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>70</v>
@@ -4112,7 +4112,7 @@
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4132,16 +4132,16 @@
         <v>55</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -4162,16 +4162,16 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -4575,13 +4575,13 @@
         <v>57</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E24" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -4793,13 +4793,13 @@
         <v>36</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>70</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -5105,7 +5105,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:L2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5127,34 +5127,34 @@
         <v>55</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="G1" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="29" t="s">
+      <c r="I1" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>114</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>118</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
@@ -5170,34 +5170,34 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -5506,7 +5506,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>6</v>
@@ -5521,7 +5521,7 @@
         <v>6</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5579,10 +5579,10 @@
         <v>91</v>
       </c>
       <c r="E13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" t="s">
         <v>107</v>
-      </c>
-      <c r="F13" t="s">
-        <v>111</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>59</v>
@@ -5594,10 +5594,10 @@
         <v>91</v>
       </c>
       <c r="J13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13" t="s">
         <v>107</v>
-      </c>
-      <c r="K13" t="s">
-        <v>111</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>59</v>
@@ -5974,31 +5974,31 @@
         <v>91</v>
       </c>
       <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
         <v>107</v>
-      </c>
-      <c r="E24" t="s">
-        <v>111</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>91</v>
       </c>
       <c r="I24" t="s">
+        <v>103</v>
+      </c>
+      <c r="J24" t="s">
         <v>107</v>
-      </c>
-      <c r="J24" t="s">
-        <v>111</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>59</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
@@ -6379,31 +6379,31 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" t="s">
         <v>107</v>
-      </c>
-      <c r="D35" t="s">
-        <v>111</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>59</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G35" s="31" t="s">
         <v>70</v>
       </c>
       <c r="H35" t="s">
+        <v>103</v>
+      </c>
+      <c r="I35" t="s">
         <v>107</v>
-      </c>
-      <c r="I35" t="s">
-        <v>111</v>
       </c>
       <c r="J35" s="16" t="s">
         <v>59</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L35" s="31" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Fixing coefficients in crop table
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS1/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS1/FieldConfigs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544B4564-2438-4D44-B766-8B313093D0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C92DF0-D59C-4389-9837-7F3515780EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="LincolnRot1" sheetId="3" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="123">
   <si>
     <t>InitialN</t>
   </si>
@@ -398,9 +398,6 @@
     <t>LincolnRot2_N1_Irr1_Oat</t>
   </si>
   <si>
-    <t>Potato Agria Maturity harvest</t>
-  </si>
-  <si>
     <t>LincolnRot2_N1_Irr1_Potato</t>
   </si>
   <si>
@@ -477,6 +474,12 @@
   </si>
   <si>
     <t>HawkesBayRot3_N1_Irr2_Ryegrass</t>
+  </si>
+  <si>
+    <t>Agria Potato Maturity harvest</t>
+  </si>
+  <si>
+    <t>LincolnActual</t>
   </si>
 </sst>
 </file>
@@ -1125,24 +1128,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A90A1-2F9B-4EC2-8DA6-AD1920316E14}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>55</v>
@@ -1173,7 +1176,7 @@
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>56</v>
       </c>
@@ -1181,31 +1184,31 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -1235,7 +1238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>71</v>
@@ -1265,7 +1268,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>73</v>
@@ -1295,7 +1298,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>74</v>
@@ -1325,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -1355,7 +1358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -1385,7 +1388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -1415,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -1445,7 +1448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -1475,7 +1478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -1506,7 +1509,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>48</v>
       </c>
@@ -1538,7 +1541,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>76</v>
@@ -1568,7 +1571,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -1598,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -1628,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -1658,7 +1661,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -1688,7 +1691,7 @@
         <v>44446</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -1718,7 +1721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -1748,7 +1751,7 @@
         <v>44623</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -1778,7 +1781,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -1808,7 +1811,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -1838,7 +1841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>49</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
         <v>80</v>
@@ -1867,11 +1870,11 @@
         <v>57</v>
       </c>
       <c r="J24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>77</v>
@@ -1901,7 +1904,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>26</v>
@@ -1928,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>27</v>
@@ -1955,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>28</v>
@@ -1985,7 +1988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>29</v>
@@ -2015,7 +2018,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>30</v>
@@ -2045,7 +2048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>31</v>
@@ -2075,7 +2078,7 @@
         <v>44933</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>32</v>
@@ -2105,7 +2108,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>34</v>
@@ -2135,7 +2138,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>35</v>
@@ -2166,7 +2169,7 @@
       </c>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>50</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -2192,13 +2195,13 @@
         <v>57</v>
       </c>
       <c r="I35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>78</v>
@@ -2228,7 +2231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>38</v>
@@ -2255,7 +2258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>39</v>
@@ -2282,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>40</v>
@@ -2312,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>41</v>
@@ -2342,7 +2345,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>42</v>
@@ -2372,7 +2375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>43</v>
@@ -2402,7 +2405,7 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>44</v>
@@ -2432,7 +2435,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>45</v>
@@ -2462,7 +2465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>46</v>
@@ -2493,8 +2496,8 @@
       </c>
       <c r="K45" s="13"/>
     </row>
-    <row r="49" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>52</v>
       </c>
@@ -2508,7 +2511,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>58</v>
       </c>
@@ -2522,7 +2525,7 @@
       <c r="J51" s="5"/>
       <c r="K51" s="6"/>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>61</v>
       </c>
@@ -2536,7 +2539,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="6"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>66</v>
       </c>
@@ -2550,7 +2553,7 @@
       <c r="J53" s="5"/>
       <c r="K53" s="6"/>
     </row>
-    <row r="54" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11" t="s">
         <v>69</v>
       </c>
@@ -2580,21 +2583,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5455F7E-3498-453E-982D-C120B5675E13}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
-    <col min="9" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>55</v>
@@ -2606,22 +2609,22 @@
         <v>94</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>100</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>101</v>
       </c>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
@@ -2630,7 +2633,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>56</v>
       </c>
@@ -2662,7 +2665,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -2692,7 +2695,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>71</v>
@@ -2722,7 +2725,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>73</v>
@@ -2752,7 +2755,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>74</v>
@@ -2782,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -2812,7 +2815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -2842,7 +2845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -2872,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -2902,7 +2905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -2932,7 +2935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -2968,7 +2971,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>48</v>
       </c>
@@ -2985,7 +2988,7 @@
         <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="G13" s="31" t="s">
         <v>70</v>
@@ -2997,10 +3000,10 @@
         <v>37</v>
       </c>
       <c r="J13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>76</v>
@@ -3030,7 +3033,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -3060,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -3090,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -3120,7 +3123,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -3150,7 +3153,7 @@
         <v>44491</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -3180,7 +3183,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -3210,7 +3213,7 @@
         <v>44629</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -3240,7 +3243,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -3270,7 +3273,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -3300,7 +3303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>49</v>
       </c>
@@ -3314,10 +3317,10 @@
         <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="F24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
         <v>91</v>
@@ -3326,10 +3329,10 @@
         <v>37</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="J24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -3338,7 +3341,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>77</v>
@@ -3368,7 +3371,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>26</v>
@@ -3398,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>27</v>
@@ -3428,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>28</v>
@@ -3458,7 +3461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>29</v>
@@ -3488,7 +3491,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>30</v>
@@ -3518,7 +3521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>31</v>
@@ -3548,7 +3551,7 @@
         <v>44933</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>32</v>
@@ -3578,7 +3581,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>34</v>
@@ -3608,7 +3611,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>35</v>
@@ -3644,7 +3647,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>50</v>
       </c>
@@ -3655,10 +3658,10 @@
         <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
@@ -3667,16 +3670,16 @@
         <v>37</v>
       </c>
       <c r="H35" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="I35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>78</v>
@@ -3706,7 +3709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>38</v>
@@ -3736,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>39</v>
@@ -3766,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>40</v>
@@ -3796,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>41</v>
@@ -3826,7 +3829,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>42</v>
@@ -3856,7 +3859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>43</v>
@@ -3886,7 +3889,7 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>44</v>
@@ -3916,7 +3919,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>45</v>
@@ -3946,7 +3949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>46</v>
@@ -3982,8 +3985,8 @@
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="49" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>52</v>
       </c>
@@ -4002,7 +4005,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>67</v>
       </c>
@@ -4021,7 +4024,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>60</v>
       </c>
@@ -4040,7 +4043,7 @@
       <c r="O52" s="5"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>63</v>
       </c>
@@ -4059,7 +4062,7 @@
       <c r="O53" s="5"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>68</v>
       </c>
@@ -4078,7 +4081,7 @@
       <c r="O54" s="5"/>
       <c r="P54" s="6"/>
     </row>
-    <row r="55" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="11"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -4115,33 +4118,33 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="15" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>120</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>121</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -4154,7 +4157,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>56</v>
       </c>
@@ -4162,19 +4165,19 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -4192,7 +4195,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>71</v>
@@ -4210,25 +4213,25 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>74</v>
@@ -4246,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -4264,7 +4267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -4282,7 +4285,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -4300,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -4318,7 +4321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -4336,7 +4339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -4364,7 +4367,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>48</v>
       </c>
@@ -4384,7 +4387,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>76</v>
@@ -4402,7 +4405,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -4420,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -4438,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -4456,7 +4459,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -4474,7 +4477,7 @@
         <v>44464</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -4492,7 +4495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -4510,7 +4513,7 @@
         <v>44602</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -4528,7 +4531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -4546,7 +4549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -4564,7 +4567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>49</v>
       </c>
@@ -4575,13 +4578,13 @@
         <v>57</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E24" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -4594,7 +4597,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>77</v>
@@ -4612,7 +4615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>26</v>
@@ -4630,7 +4633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>27</v>
@@ -4648,7 +4651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>28</v>
@@ -4666,7 +4669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>29</v>
@@ -4685,7 +4688,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>30</v>
@@ -4703,7 +4706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>31</v>
@@ -4721,7 +4724,7 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>32</v>
@@ -4739,7 +4742,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>34</v>
@@ -4757,7 +4760,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>35</v>
@@ -4785,7 +4788,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>50</v>
       </c>
@@ -4793,19 +4796,19 @@
         <v>36</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>70</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>78</v>
@@ -4823,7 +4826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>38</v>
@@ -4841,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>39</v>
@@ -4859,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>40</v>
@@ -4877,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>41</v>
@@ -4895,7 +4898,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>42</v>
@@ -4914,7 +4917,7 @@
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>43</v>
@@ -4932,7 +4935,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>44</v>
@@ -4950,7 +4953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>45</v>
@@ -4968,7 +4971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>46</v>
@@ -4996,8 +4999,8 @@
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="49" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>52</v>
       </c>
@@ -5016,7 +5019,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>62</v>
       </c>
@@ -5035,7 +5038,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>63</v>
       </c>
@@ -5054,7 +5057,7 @@
       <c r="O52" s="5"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -5071,7 +5074,7 @@
       <c r="O53" s="5"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
@@ -5104,57 +5107,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B8B917-5635-4965-8A45-89E9AEAAEA05}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="6" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37" style="15" customWidth="1"/>
-    <col min="10" max="11" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.33203125" style="15" customWidth="1"/>
+    <col min="10" max="11" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>105</v>
-      </c>
       <c r="F1" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>113</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>114</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
@@ -5162,7 +5165,7 @@
       <c r="P1" s="13"/>
       <c r="Q1" s="13"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>56</v>
       </c>
@@ -5170,37 +5173,37 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -5236,7 +5239,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>71</v>
@@ -5272,43 +5275,43 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>74</v>
@@ -5344,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -5380,7 +5383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -5416,7 +5419,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -5452,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -5488,7 +5491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -5506,7 +5509,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>6</v>
@@ -5521,10 +5524,10 @@
         <v>6</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -5565,7 +5568,7 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>48</v>
       </c>
@@ -5579,10 +5582,10 @@
         <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>59</v>
@@ -5594,16 +5597,16 @@
         <v>91</v>
       </c>
       <c r="J13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>76</v>
@@ -5639,7 +5642,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -5675,7 +5678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -5711,7 +5714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -5747,7 +5750,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -5783,7 +5786,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -5819,7 +5822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -5855,7 +5858,7 @@
         <v>44852</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -5891,7 +5894,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -5927,7 +5930,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -5963,7 +5966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>49</v>
       </c>
@@ -5974,31 +5977,31 @@
         <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>91</v>
       </c>
       <c r="I24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>59</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
@@ -6006,7 +6009,7 @@
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>77</v>
@@ -6042,7 +6045,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>26</v>
@@ -6078,7 +6081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>27</v>
@@ -6114,7 +6117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>28</v>
@@ -6150,7 +6153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>29</v>
@@ -6186,7 +6189,7 @@
         <v>45056</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>30</v>
@@ -6222,7 +6225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>31</v>
@@ -6258,7 +6261,7 @@
         <v>45298</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>32</v>
@@ -6294,7 +6297,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>34</v>
@@ -6330,7 +6333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>35</v>
@@ -6371,7 +6374,7 @@
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>50</v>
       </c>
@@ -6379,37 +6382,37 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>59</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G35" s="31" t="s">
         <v>70</v>
       </c>
       <c r="H35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J35" s="16" t="s">
         <v>59</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L35" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>78</v>
@@ -6445,7 +6448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>38</v>
@@ -6481,7 +6484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>39</v>
@@ -6517,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>40</v>
@@ -6553,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>41</v>
@@ -6589,7 +6592,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>42</v>
@@ -6625,7 +6628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>43</v>
@@ -6661,7 +6664,7 @@
         <v>45505</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>44</v>
@@ -6697,7 +6700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>45</v>
@@ -6733,7 +6736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>46</v>
@@ -6774,8 +6777,8 @@
       <c r="P45" s="13"/>
       <c r="Q45" s="13"/>
     </row>
-    <row r="49" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>52</v>
       </c>
@@ -6795,7 +6798,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="3"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
@@ -6813,7 +6816,7 @@
       <c r="P51" s="5"/>
       <c r="Q51" s="6"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
@@ -6831,7 +6834,7 @@
       <c r="P52" s="5"/>
       <c r="Q52" s="6"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -6849,7 +6852,7 @@
       <c r="P53" s="5"/>
       <c r="Q53" s="6"/>
     </row>
-    <row r="54" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>

</xml_diff>

<commit_message>
tidy up configs for WS1
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS1/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS1/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C92DF0-D59C-4389-9837-7F3515780EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE8337C-A352-4425-965F-7CF7051E621C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="LincolnRot1" sheetId="3" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="118">
   <si>
     <t>InitialN</t>
   </si>
@@ -188,9 +188,6 @@
     <t>CurrentCropNameFull</t>
   </si>
   <si>
-    <t>Potato Vegetable General</t>
-  </si>
-  <si>
     <t>CurrentFieldLoss</t>
   </si>
   <si>
@@ -350,9 +347,6 @@
     <t>FollowingFieldYield</t>
   </si>
   <si>
-    <t>lincoln</t>
-  </si>
-  <si>
     <t>Wheat Grain Feed</t>
   </si>
   <si>
@@ -368,9 +362,6 @@
     <t>LincolnRot1_N1_Irr1_Onion</t>
   </si>
   <si>
-    <t>Bailed</t>
-  </si>
-  <si>
     <t>LincolnRot1_N1_Irr1_Ryegrass</t>
   </si>
   <si>
@@ -437,9 +428,6 @@
     <t>HawkesBayRot4_N1_Irr1_Cauliflower</t>
   </si>
   <si>
-    <t>HawkesBayRot4_N1_Irr1_Ryegrass</t>
-  </si>
-  <si>
     <t>HawkesBayRot4_N1_Irr2_PakChoi</t>
   </si>
   <si>
@@ -452,18 +440,9 @@
     <t>HawkesBayRot4_N1_Irr2_Cauliflower</t>
   </si>
   <si>
-    <t>HawkesBayRot4_N1_Irr2_Ryegrass</t>
-  </si>
-  <si>
     <t>Ryegrass Seed General</t>
   </si>
   <si>
-    <t>Very Wet</t>
-  </si>
-  <si>
-    <t>hastings</t>
-  </si>
-  <si>
     <t>HawkesBayRot3_N1_Irr1_Onion</t>
   </si>
   <si>
@@ -476,10 +455,16 @@
     <t>HawkesBayRot3_N1_Irr2_Ryegrass</t>
   </si>
   <si>
-    <t>Agria Potato Maturity harvest</t>
-  </si>
-  <si>
     <t>LincolnActual</t>
+  </si>
+  <si>
+    <t>Maturity harvest Potato RussetBurbank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maturity harvest Potato Agria </t>
+  </si>
+  <si>
+    <t>HastingsActual</t>
   </si>
 </sst>
 </file>
@@ -1128,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A90A1-2F9B-4EC2-8DA6-AD1920316E14}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,64 +1133,64 @@
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>90</v>
       </c>
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="H2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1241,67 +1226,67 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1484,16 +1469,16 @@
         <v>8</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>9</v>
@@ -1511,40 +1496,40 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" t="s">
-        <v>82</v>
-      </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="H13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" t="s">
         <v>80</v>
       </c>
-      <c r="I13" t="s">
-        <v>82</v>
-      </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="25">
         <v>70</v>
@@ -1703,7 +1688,7 @@
         <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
         <v>16</v>
@@ -1715,7 +1700,7 @@
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
@@ -1757,28 +1742,28 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I21" t="s">
         <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1790,7 +1775,7 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
         <v>21</v>
@@ -1802,7 +1787,7 @@
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I22" t="s">
         <v>21</v>
@@ -1843,41 +1828,41 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
         <v>80</v>
       </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" t="s">
         <v>80</v>
       </c>
-      <c r="H24" t="s">
-        <v>82</v>
-      </c>
       <c r="I24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="27">
         <v>10.3</v>
@@ -1907,7 +1892,7 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1934,7 +1919,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1961,7 +1946,7 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>14</v>
@@ -1991,7 +1976,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1">
         <v>43969</v>
@@ -2021,13 +2006,13 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
@@ -2039,7 +2024,7 @@
         <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I30" t="s">
         <v>16</v>
@@ -2051,7 +2036,7 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>44218</v>
@@ -2081,40 +2066,40 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H32" t="s">
         <v>19</v>
       </c>
       <c r="I32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
@@ -2123,10 +2108,10 @@
         <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H33" t="s">
         <v>21</v>
@@ -2135,13 +2120,13 @@
         <v>21</v>
       </c>
       <c r="J33" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>23</v>
@@ -2171,40 +2156,40 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I35" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J35" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>16</v>
@@ -2234,7 +2219,7 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2261,7 +2246,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2288,7 +2273,7 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>89</v>
@@ -2318,7 +2303,7 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="1">
         <v>44258</v>
@@ -2348,10 +2333,10 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
         <v>16</v>
@@ -2363,7 +2348,7 @@
         <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H41" t="s">
         <v>16</v>
@@ -2378,7 +2363,7 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1">
         <v>44379</v>
@@ -2390,7 +2375,7 @@
         <v>44933</v>
       </c>
       <c r="F42" s="32">
-        <v>45170</v>
+        <v>45072</v>
       </c>
       <c r="G42" s="1">
         <v>44379</v>
@@ -2402,22 +2387,22 @@
         <v>44933</v>
       </c>
       <c r="J42" s="32">
-        <v>45170</v>
+        <v>45072</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>19</v>
@@ -2426,10 +2411,10 @@
         <v>19</v>
       </c>
       <c r="H43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J43" s="31" t="s">
         <v>19</v>
@@ -2438,7 +2423,7 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
         <v>21</v>
@@ -2447,7 +2432,7 @@
         <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F44" s="31" t="s">
         <v>21</v>
@@ -2459,7 +2444,7 @@
         <v>21</v>
       </c>
       <c r="I44" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="J44" s="31" t="s">
         <v>21</v>
@@ -2468,7 +2453,7 @@
     <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>23</v>
@@ -2499,7 +2484,7 @@
     <row r="49" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -2513,7 +2498,7 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -2527,7 +2512,7 @@
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2541,7 +2526,7 @@
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -2555,7 +2540,7 @@
     </row>
     <row r="54" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -2583,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5455F7E-3498-453E-982D-C120B5675E13}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,31 +2585,31 @@
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
@@ -2635,34 +2620,34 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2698,67 +2683,67 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2941,16 +2926,16 @@
         <v>8</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>9</v>
@@ -2973,40 +2958,40 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="31">
         <v>3</v>
@@ -3222,25 +3207,25 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G21" s="31" t="s">
         <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3305,34 +3290,34 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I24" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="J24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -3344,7 +3329,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <v>59</v>
@@ -3374,7 +3359,7 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -3404,7 +3389,7 @@
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -3434,7 +3419,7 @@
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>94</v>
@@ -3464,7 +3449,7 @@
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1">
         <v>44172</v>
@@ -3494,7 +3479,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
@@ -3524,7 +3509,7 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>44219</v>
@@ -3554,37 +3539,37 @@
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
@@ -3596,7 +3581,7 @@
         <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
         <v>21</v>
@@ -3608,13 +3593,13 @@
         <v>21</v>
       </c>
       <c r="J33" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>23</v>
@@ -3649,40 +3634,40 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
         <v>36</v>
       </c>
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
       <c r="D35" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H35" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I35" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J35" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>7.5</v>
@@ -3712,7 +3697,7 @@
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -3742,7 +3727,7 @@
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -3772,7 +3757,7 @@
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3802,7 +3787,7 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="1">
         <v>44257</v>
@@ -3832,7 +3817,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
@@ -3862,7 +3847,7 @@
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1">
         <v>44407</v>
@@ -3874,7 +3859,7 @@
         <v>44933</v>
       </c>
       <c r="F42" s="32">
-        <v>45170</v>
+        <v>45072</v>
       </c>
       <c r="G42" s="1">
         <v>44407</v>
@@ -3886,34 +3871,34 @@
         <v>44933</v>
       </c>
       <c r="J42" s="32">
-        <v>45170</v>
+        <v>45072</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J43" s="31" t="s">
         <v>19</v>
@@ -3922,7 +3907,7 @@
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
         <v>21</v>
@@ -3931,7 +3916,7 @@
         <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F44" s="31" t="s">
         <v>21</v>
@@ -3943,7 +3928,7 @@
         <v>21</v>
       </c>
       <c r="I44" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="J44" s="31" t="s">
         <v>21</v>
@@ -3952,7 +3937,7 @@
     <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>23</v>
@@ -3988,7 +3973,7 @@
     <row r="49" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="2"/>
@@ -4007,7 +3992,7 @@
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="5"/>
@@ -4026,7 +4011,7 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -4045,7 +4030,7 @@
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -4064,7 +4049,7 @@
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -4114,8 +4099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AD42EA-A0EE-4986-A449-DEBA14E52DE4}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4132,19 +4117,19 @@
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -4159,22 +4144,22 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -4198,43 +4183,43 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>72</v>
-      </c>
       <c r="D4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="16">
         <v>0</v>
@@ -4345,10 +4330,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>9</v>
@@ -4369,28 +4354,28 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="31">
         <v>3</v>
@@ -4522,13 +4507,13 @@
         <v>19</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -4569,22 +4554,22 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -4600,7 +4585,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="16">
         <v>44</v>
@@ -4618,7 +4603,7 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="16">
         <v>0</v>
@@ -4636,7 +4621,7 @@
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="16">
         <v>0</v>
@@ -4654,7 +4639,7 @@
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="16">
         <v>87</v>
@@ -4672,7 +4657,7 @@
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="17">
         <v>44464</v>
@@ -4691,7 +4676,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>16</v>
@@ -4709,7 +4694,7 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="17">
         <v>44602</v>
@@ -4727,43 +4712,43 @@
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>21</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>23</v>
@@ -4790,28 +4775,28 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" s="16">
         <v>1</v>
@@ -4829,7 +4814,7 @@
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="16">
         <v>0</v>
@@ -4847,7 +4832,7 @@
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" s="16">
         <v>0</v>
@@ -4865,7 +4850,7 @@
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" s="16">
         <v>14</v>
@@ -4883,7 +4868,7 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="17">
         <v>44640</v>
@@ -4901,7 +4886,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>16</v>
@@ -4920,34 +4905,34 @@
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="17">
         <v>44895</v>
       </c>
-      <c r="D42" s="32">
-        <v>45139</v>
+      <c r="D42" s="17">
+        <v>45072</v>
       </c>
       <c r="E42" s="17">
         <v>44895</v>
       </c>
-      <c r="F42" s="32">
-        <v>45139</v>
+      <c r="F42" s="17">
+        <v>45072</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>19</v>
@@ -4956,16 +4941,16 @@
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D44" s="31" t="s">
         <v>21</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F44" s="31" t="s">
         <v>21</v>
@@ -4974,7 +4959,7 @@
     <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>23</v>
@@ -5002,7 +4987,7 @@
     <row r="49" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="20"/>
@@ -5021,7 +5006,7 @@
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
@@ -5040,7 +5025,7 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
@@ -5105,10 +5090,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B8B917-5635-4965-8A45-89E9AEAAEA05}">
-  <dimension ref="A1:Q54"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5116,94 +5101,79 @@
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="6" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37" style="15" customWidth="1"/>
-    <col min="10" max="11" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.28515625" style="15" customWidth="1"/>
+    <col min="5" max="7" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37" style="15" customWidth="1"/>
+    <col min="9" max="10" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D1" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="29" t="s">
+      <c r="H1" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>113</v>
-      </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -5232,89 +5202,71 @@
       <c r="J3" s="15">
         <v>50</v>
       </c>
-      <c r="K3" s="15">
-        <v>50</v>
-      </c>
-      <c r="L3" s="15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>72</v>
-      </c>
       <c r="D4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="16">
         <v>0</v>
@@ -5340,14 +5292,8 @@
       <c r="J6" s="16">
         <v>0</v>
       </c>
-      <c r="K6" s="16">
-        <v>0</v>
-      </c>
-      <c r="L6" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -5376,14 +5322,8 @@
       <c r="J7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -5412,14 +5352,8 @@
       <c r="J8" s="25">
         <v>85</v>
       </c>
-      <c r="K8" s="25">
-        <v>85</v>
-      </c>
-      <c r="L8" s="25">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -5448,14 +5382,8 @@
       <c r="J9" s="16">
         <v>0</v>
       </c>
-      <c r="K9" s="16">
-        <v>0</v>
-      </c>
-      <c r="L9" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -5484,14 +5412,8 @@
       <c r="J10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -5509,7 +5431,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>6</v>
@@ -5520,96 +5442,78 @@
       <c r="J11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>64</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
+        <v>99</v>
       </c>
       <c r="J13" t="s">
-        <v>102</v>
-      </c>
-      <c r="K13" t="s">
-        <v>106</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="18">
         <v>8</v>
@@ -5623,26 +5527,20 @@
       <c r="F14" s="16">
         <v>8</v>
       </c>
-      <c r="G14" s="25">
-        <v>46</v>
-      </c>
-      <c r="H14" s="18">
+      <c r="G14" s="18">
         <v>8</v>
       </c>
+      <c r="H14" s="16">
+        <v>61</v>
+      </c>
       <c r="I14" s="16">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J14" s="16">
-        <v>53</v>
-      </c>
-      <c r="K14" s="16">
         <v>8</v>
       </c>
-      <c r="L14" s="25">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -5659,10 +5557,10 @@
       <c r="F15" s="16">
         <v>0</v>
       </c>
-      <c r="G15" s="16">
-        <v>0</v>
-      </c>
-      <c r="H15" s="25">
+      <c r="G15" s="25">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16">
         <v>0</v>
       </c>
       <c r="I15" s="16">
@@ -5671,14 +5569,8 @@
       <c r="J15" s="16">
         <v>0</v>
       </c>
-      <c r="K15" s="16">
-        <v>0</v>
-      </c>
-      <c r="L15" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -5695,10 +5587,10 @@
       <c r="F16" s="16">
         <v>0</v>
       </c>
-      <c r="G16" s="16">
-        <v>0</v>
-      </c>
-      <c r="H16" s="25">
+      <c r="G16" s="25">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16">
         <v>0</v>
       </c>
       <c r="I16" s="16">
@@ -5707,14 +5599,8 @@
       <c r="J16" s="16">
         <v>0</v>
       </c>
-      <c r="K16" s="16">
-        <v>0</v>
-      </c>
-      <c r="L16" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -5731,26 +5617,20 @@
       <c r="F17" s="16">
         <v>78</v>
       </c>
-      <c r="G17" s="25">
-        <v>94</v>
-      </c>
-      <c r="H17" s="18">
-        <v>0</v>
+      <c r="G17" s="18">
+        <v>0</v>
+      </c>
+      <c r="H17" s="16">
+        <v>95</v>
       </c>
       <c r="I17" s="16">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J17" s="16">
-        <v>97</v>
-      </c>
-      <c r="K17" s="16">
         <v>78</v>
       </c>
-      <c r="L17" s="25">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -5767,26 +5647,20 @@
       <c r="F18" s="17">
         <v>44550</v>
       </c>
-      <c r="G18" s="17">
-        <v>44693</v>
-      </c>
-      <c r="H18" s="30">
+      <c r="G18" s="30">
         <v>44013</v>
       </c>
+      <c r="H18" s="17">
+        <v>44308</v>
+      </c>
       <c r="I18" s="17">
-        <v>44308</v>
+        <v>44448</v>
       </c>
       <c r="J18" s="17">
-        <v>44448</v>
-      </c>
-      <c r="K18" s="17">
         <v>44550</v>
       </c>
-      <c r="L18" s="17">
-        <v>44693</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -5798,7 +5672,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>16</v>
@@ -5810,19 +5684,13 @@
         <v>16</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -5839,26 +5707,20 @@
       <c r="F20" s="17">
         <v>44614</v>
       </c>
-      <c r="G20" s="17">
-        <v>44852</v>
-      </c>
-      <c r="H20" s="30">
+      <c r="G20" s="30">
         <v>44136</v>
       </c>
+      <c r="H20" s="17">
+        <v>44386</v>
+      </c>
       <c r="I20" s="17">
-        <v>44386</v>
+        <v>44520</v>
       </c>
       <c r="J20" s="17">
-        <v>44520</v>
-      </c>
-      <c r="K20" s="17">
         <v>44614</v>
       </c>
-      <c r="L20" s="17">
-        <v>44852</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -5867,34 +5729,28 @@
         <v>19</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -5923,14 +5779,8 @@
       <c r="J22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -5959,60 +5809,48 @@
       <c r="J23" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="H24" t="s">
+        <v>99</v>
       </c>
       <c r="I24" t="s">
-        <v>102</v>
-      </c>
-      <c r="J24" t="s">
-        <v>106</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>114</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="16">
         <v>61</v>
@@ -6026,29 +5864,23 @@
       <c r="F25" s="25">
         <v>46</v>
       </c>
-      <c r="G25" s="25">
-        <v>1.5</v>
+      <c r="G25" s="16">
+        <v>61</v>
       </c>
       <c r="H25" s="16">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I25" s="16">
-        <v>53</v>
-      </c>
-      <c r="J25" s="16">
         <v>8</v>
       </c>
-      <c r="K25" s="25">
+      <c r="J25" s="25">
         <v>46</v>
       </c>
-      <c r="L25" s="25">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="16">
         <v>0</v>
@@ -6074,17 +5906,11 @@
       <c r="J26" s="16">
         <v>0</v>
       </c>
-      <c r="K26" s="16">
-        <v>0</v>
-      </c>
-      <c r="L26" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="16">
         <v>0</v>
@@ -6110,17 +5936,11 @@
       <c r="J27" s="16">
         <v>0</v>
       </c>
-      <c r="K27" s="16">
-        <v>0</v>
-      </c>
-      <c r="L27" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="16">
         <v>95</v>
@@ -6135,28 +5955,22 @@
         <v>94</v>
       </c>
       <c r="G28" s="16">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="H28" s="16">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I28" s="16">
-        <v>97</v>
-      </c>
-      <c r="J28" s="16">
         <v>78</v>
       </c>
-      <c r="K28" s="25">
+      <c r="J28" s="25">
         <v>94</v>
       </c>
-      <c r="L28" s="16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="17">
         <v>44308</v>
@@ -6171,34 +5985,28 @@
         <v>44693</v>
       </c>
       <c r="G29" s="17">
-        <v>45056</v>
+        <v>44308</v>
       </c>
       <c r="H29" s="17">
-        <v>44308</v>
+        <v>44448</v>
       </c>
       <c r="I29" s="17">
-        <v>44448</v>
+        <v>44550</v>
       </c>
       <c r="J29" s="17">
-        <v>44550</v>
-      </c>
-      <c r="K29" s="17">
         <v>44693</v>
       </c>
-      <c r="L29" s="17">
-        <v>45056</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>16</v>
@@ -6210,25 +6018,19 @@
         <v>16</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="J30" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="17">
         <v>44386</v>
@@ -6243,64 +6045,52 @@
         <v>44852</v>
       </c>
       <c r="G31" s="17">
-        <v>45298</v>
+        <v>44386</v>
       </c>
       <c r="H31" s="17">
-        <v>44386</v>
+        <v>44520</v>
       </c>
       <c r="I31" s="17">
-        <v>44520</v>
+        <v>44614</v>
       </c>
       <c r="J31" s="17">
-        <v>44614</v>
-      </c>
-      <c r="K31" s="17">
         <v>44852</v>
       </c>
-      <c r="L31" s="17">
-        <v>45298</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>33</v>
-      </c>
       <c r="F32" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>21</v>
@@ -6326,17 +6116,11 @@
       <c r="J33" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K33" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>23</v>
@@ -6362,60 +6146,48 @@
       <c r="J34" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L34" s="23" t="s">
-        <v>23</v>
-      </c>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="G35" s="31" t="s">
-        <v>70</v>
+        <v>109</v>
+      </c>
+      <c r="G35" t="s">
+        <v>99</v>
       </c>
       <c r="H35" t="s">
-        <v>102</v>
-      </c>
-      <c r="I35" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="L35" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" s="16">
         <v>53</v>
@@ -6429,29 +6201,23 @@
       <c r="F36" s="25">
         <v>1.5</v>
       </c>
-      <c r="G36" s="31">
-        <v>3</v>
+      <c r="G36" s="16">
+        <v>53</v>
       </c>
       <c r="H36" s="16">
-        <v>53</v>
-      </c>
-      <c r="I36" s="16">
         <v>8</v>
       </c>
+      <c r="I36" s="25">
+        <v>46</v>
+      </c>
       <c r="J36" s="25">
-        <v>46</v>
-      </c>
-      <c r="K36" s="25">
         <v>1.5</v>
       </c>
-      <c r="L36" s="31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="16">
         <v>0</v>
@@ -6465,7 +6231,7 @@
       <c r="F37" s="16">
         <v>0</v>
       </c>
-      <c r="G37" s="31">
+      <c r="G37" s="16">
         <v>0</v>
       </c>
       <c r="H37" s="16">
@@ -6477,17 +6243,11 @@
       <c r="J37" s="16">
         <v>0</v>
       </c>
-      <c r="K37" s="16">
-        <v>0</v>
-      </c>
-      <c r="L37" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" s="16">
         <v>0</v>
@@ -6501,7 +6261,7 @@
       <c r="F38" s="16">
         <v>0</v>
       </c>
-      <c r="G38" s="31">
+      <c r="G38" s="16">
         <v>0</v>
       </c>
       <c r="H38" s="16">
@@ -6513,17 +6273,11 @@
       <c r="J38" s="16">
         <v>0</v>
       </c>
-      <c r="K38" s="16">
-        <v>0</v>
-      </c>
-      <c r="L38" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" s="16">
         <v>97</v>
@@ -6537,29 +6291,23 @@
       <c r="F39" s="16">
         <v>14</v>
       </c>
-      <c r="G39" s="31">
-        <v>0</v>
+      <c r="G39" s="16">
+        <v>97</v>
       </c>
       <c r="H39" s="16">
-        <v>97</v>
-      </c>
-      <c r="I39" s="16">
         <v>78</v>
       </c>
-      <c r="J39" s="25">
+      <c r="I39" s="25">
         <v>94</v>
       </c>
-      <c r="K39" s="16">
+      <c r="J39" s="16">
         <v>14</v>
       </c>
-      <c r="L39" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="17">
         <v>44448</v>
@@ -6573,32 +6321,26 @@
       <c r="F40" s="17">
         <v>45056</v>
       </c>
-      <c r="G40" s="32">
-        <v>45352</v>
+      <c r="G40" s="17">
+        <v>44448</v>
       </c>
       <c r="H40" s="17">
-        <v>44448</v>
+        <v>44550</v>
       </c>
       <c r="I40" s="17">
-        <v>44550</v>
+        <v>44693</v>
       </c>
       <c r="J40" s="17">
-        <v>44693</v>
-      </c>
-      <c r="K40" s="17">
         <v>45056</v>
       </c>
-      <c r="L40" s="32">
-        <v>45352</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" s="16" t="s">
         <v>16</v>
@@ -6609,11 +6351,11 @@
       <c r="F41" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="31" t="s">
-        <v>16</v>
+      <c r="G41" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="I41" s="16" t="s">
         <v>16</v>
@@ -6621,17 +6363,11 @@
       <c r="J41" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K41" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L41" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="17">
         <v>44520</v>
@@ -6643,67 +6379,55 @@
         <v>44852</v>
       </c>
       <c r="F42" s="17">
-        <v>45298</v>
-      </c>
-      <c r="G42" s="32">
-        <v>45505</v>
+        <v>45072</v>
+      </c>
+      <c r="G42" s="17">
+        <v>44520</v>
       </c>
       <c r="H42" s="17">
-        <v>44520</v>
+        <v>44614</v>
       </c>
       <c r="I42" s="17">
-        <v>44614</v>
+        <v>44852</v>
       </c>
       <c r="J42" s="17">
-        <v>44852</v>
-      </c>
-      <c r="K42" s="17">
-        <v>45298</v>
-      </c>
-      <c r="L42" s="32">
-        <v>45505</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>45072</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G43" s="31" t="s">
-        <v>19</v>
+        <v>50</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="K43" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L43" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>21</v>
@@ -6717,7 +6441,7 @@
       <c r="F44" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G44" s="31" t="s">
+      <c r="G44" s="16" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="16" t="s">
@@ -6729,17 +6453,11 @@
       <c r="J44" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K44" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="L44" s="31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>23</v>
@@ -6753,7 +6471,7 @@
       <c r="F45" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G45" s="33" t="s">
+      <c r="G45" s="23" t="s">
         <v>23</v>
       </c>
       <c r="H45" s="23" t="s">
@@ -6765,40 +6483,32 @@
       <c r="J45" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K45" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L45" s="33" t="s">
-        <v>23</v>
-      </c>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
       <c r="M45" s="13"/>
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-    </row>
-    <row r="49" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="3"/>
-    </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O50" s="3"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
@@ -6808,15 +6518,13 @@
       <c r="H51" s="21"/>
       <c r="I51" s="21"/>
       <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="6"/>
-    </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O51" s="6"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
@@ -6826,15 +6534,13 @@
       <c r="H52" s="21"/>
       <c r="I52" s="21"/>
       <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="6"/>
-    </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O52" s="6"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -6844,15 +6550,13 @@
       <c r="H53" s="21"/>
       <c r="I53" s="21"/>
       <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="21"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="6"/>
-    </row>
-    <row r="54" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O53" s="6"/>
+    </row>
+    <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
@@ -6862,13 +6566,11 @@
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
       <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="22"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="8"/>
+      <c r="O54" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Some changes to WS1 test configs and results
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS1/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS1/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B9BCAB-EDAB-4F81-8F49-C57334FD579C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649CEAE-C9FA-4EC0-8994-D13A765E5F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="LincolnRot1" sheetId="3" r:id="rId1"/>
@@ -1113,24 +1113,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A90A1-2F9B-4EC2-8DA6-AD1920316E14}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -1223,7 +1223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -1253,7 +1253,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -1283,7 +1283,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -1313,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -1343,7 +1343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -1373,7 +1373,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -1403,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -1433,7 +1433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -1463,7 +1463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -1556,7 +1556,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -1616,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -1646,7 +1646,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -1676,7 +1676,7 @@
         <v>44446</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -1706,7 +1706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -1736,7 +1736,7 @@
         <v>44623</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -1766,7 +1766,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -1796,7 +1796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -1826,7 +1826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -1889,7 +1889,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -1973,7 +1973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -2003,7 +2003,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -2033,7 +2033,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -2063,7 +2063,7 @@
         <v>44933</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -2093,7 +2093,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -2123,7 +2123,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -2216,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -2270,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -2330,7 +2330,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -2360,7 +2360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -2390,7 +2390,7 @@
         <v>45072</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -2420,7 +2420,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -2450,7 +2450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -2481,8 +2481,8 @@
       </c>
       <c r="K45" s="13"/>
     </row>
-    <row r="49" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
         <v>56</v>
       </c>
@@ -2510,7 +2510,7 @@
       <c r="J51" s="5"/>
       <c r="K51" s="6"/>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
         <v>59</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="6"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="4" t="s">
         <v>64</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="J53" s="5"/>
       <c r="K53" s="6"/>
     </row>
-    <row r="54" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="11" t="s">
         <v>67</v>
       </c>
@@ -2568,21 +2568,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5455F7E-3498-453E-982D-C120B5675E13}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
-    <col min="9" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -2618,7 +2618,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -2680,7 +2680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -2710,7 +2710,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -2740,7 +2740,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -2800,7 +2800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -2830,7 +2830,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -2860,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -2890,7 +2890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -2920,7 +2920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -2956,7 +2956,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -3018,7 +3018,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -3078,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -3108,7 +3108,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -3138,7 +3138,7 @@
         <v>44491</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -3168,7 +3168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -3198,7 +3198,7 @@
         <v>44629</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -3228,7 +3228,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -3258,7 +3258,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -3288,7 +3288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -3326,7 +3326,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -3356,7 +3356,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -3386,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -3446,7 +3446,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -3476,7 +3476,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -3506,7 +3506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -3536,7 +3536,7 @@
         <v>44933</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -3566,7 +3566,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -3596,7 +3596,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -3632,7 +3632,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -3694,7 +3694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -3724,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -3754,7 +3754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -3784,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -3814,7 +3814,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -3844,7 +3844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -3874,7 +3874,7 @@
         <v>45072</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -3904,7 +3904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -3934,7 +3934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -3970,8 +3970,8 @@
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="49" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
         <v>65</v>
       </c>
@@ -4009,7 +4009,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
         <v>58</v>
       </c>
@@ -4028,7 +4028,7 @@
       <c r="O52" s="5"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B53" s="4" t="s">
         <v>61</v>
       </c>
@@ -4047,7 +4047,7 @@
       <c r="O53" s="5"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B54" s="4" t="s">
         <v>66</v>
       </c>
@@ -4066,7 +4066,7 @@
       <c r="O54" s="5"/>
       <c r="P54" s="6"/>
     </row>
-    <row r="55" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="11"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -4099,22 +4099,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AD42EA-A0EE-4986-A449-DEBA14E52DE4}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="15" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -4142,7 +4142,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -4180,7 +4180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -4198,7 +4198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -4216,7 +4216,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -4234,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -4252,7 +4252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -4270,7 +4270,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -4288,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -4306,7 +4306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -4324,7 +4324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -4352,7 +4352,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -4390,7 +4390,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -4408,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -4426,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -4444,7 +4444,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -4462,7 +4462,7 @@
         <v>44464</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -4480,7 +4480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -4498,7 +4498,7 @@
         <v>44602</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -4516,7 +4516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -4534,7 +4534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -4552,7 +4552,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -4582,7 +4582,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -4600,7 +4600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -4618,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -4636,7 +4636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -4654,7 +4654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -4673,7 +4673,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -4691,7 +4691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -4709,7 +4709,7 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -4727,7 +4727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -4745,7 +4745,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -4773,7 +4773,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -4811,7 +4811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -4829,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -4847,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -4865,7 +4865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -4883,7 +4883,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -4920,7 +4920,7 @@
         <v>45072</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -4938,7 +4938,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -4956,7 +4956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -4984,8 +4984,8 @@
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="49" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
@@ -5004,7 +5004,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
         <v>60</v>
       </c>
@@ -5023,7 +5023,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
         <v>61</v>
       </c>
@@ -5042,7 +5042,7 @@
       <c r="O52" s="5"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -5059,7 +5059,7 @@
       <c r="O53" s="5"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
@@ -5092,21 +5092,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B8B917-5635-4965-8A45-89E9AEAAEA05}">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="7" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" style="15" customWidth="1"/>
-    <col min="9" max="10" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -5141,7 +5141,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -5203,7 +5203,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -5233,7 +5233,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -5263,7 +5263,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -5293,7 +5293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -5323,7 +5323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -5353,7 +5353,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -5383,7 +5383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -5413,7 +5413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -5443,7 +5443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -5478,7 +5478,7 @@
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -5540,7 +5540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -5570,7 +5570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -5600,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -5630,7 +5630,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -5660,7 +5660,7 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -5690,7 +5690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -5720,7 +5720,7 @@
         <v>44614</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -5750,7 +5750,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -5780,7 +5780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -5810,7 +5810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -5847,7 +5847,7 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -5877,7 +5877,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -5907,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -5937,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -5967,7 +5967,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -5997,7 +5997,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -6027,7 +6027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -6057,7 +6057,7 @@
         <v>44852</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -6087,7 +6087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -6117,7 +6117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -6152,7 +6152,7 @@
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -6214,7 +6214,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -6244,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -6274,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -6304,7 +6304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -6334,7 +6334,7 @@
         <v>45056</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -6364,7 +6364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -6394,7 +6394,7 @@
         <v>45072</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -6424,7 +6424,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -6454,7 +6454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -6489,8 +6489,8 @@
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
     </row>
-    <row r="49" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
@@ -6508,7 +6508,7 @@
       <c r="N50" s="2"/>
       <c r="O50" s="3"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
@@ -6524,7 +6524,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="6"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
@@ -6540,7 +6540,7 @@
       <c r="N52" s="5"/>
       <c r="O52" s="6"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -6556,7 +6556,7 @@
       <c r="N53" s="5"/>
       <c r="O53" s="6"/>
     </row>
-    <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>

</xml_diff>

<commit_message>
More tidying up of test configurations
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS1/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS1/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649CEAE-C9FA-4EC0-8994-D13A765E5F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933A0FD9-9356-4F85-B06D-34E5110CEF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="LincolnRot1" sheetId="3" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="124">
   <si>
     <t>InitialN</t>
   </si>
@@ -465,6 +465,24 @@
   </si>
   <si>
     <t>Onion Vegetable Brown</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr1_RyegrassRegrowth1</t>
+  </si>
+  <si>
+    <t>Pasture Regrowth</t>
+  </si>
+  <si>
+    <t>None (Surface)</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr1_RyegrassRegrowth2</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr2_RyegrassRegrowth1</t>
+  </si>
+  <si>
+    <t>HawkesBayRot3_N1_Irr2_RyegrassRegrowth2</t>
   </si>
 </sst>
 </file>
@@ -1117,20 +1135,20 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -1161,7 +1179,7 @@
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -1193,7 +1211,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -1223,7 +1241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -1253,7 +1271,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -1283,7 +1301,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -1313,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -1343,7 +1361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -1373,7 +1391,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -1403,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -1433,7 +1451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -1463,7 +1481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -1494,7 +1512,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -1526,7 +1544,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -1556,7 +1574,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -1586,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -1616,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -1646,7 +1664,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -1676,7 +1694,7 @@
         <v>44446</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -1706,7 +1724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -1736,7 +1754,7 @@
         <v>44623</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -1766,7 +1784,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -1796,7 +1814,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -1826,7 +1844,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -1859,7 +1877,7 @@
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -1889,7 +1907,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -1916,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -1943,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -1973,7 +1991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -2003,7 +2021,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -2033,7 +2051,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -2063,7 +2081,7 @@
         <v>44933</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -2093,7 +2111,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -2123,7 +2141,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -2154,7 +2172,7 @@
       </c>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -2186,7 +2204,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -2216,7 +2234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -2243,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -2270,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -2300,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -2330,7 +2348,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -2360,7 +2378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -2390,7 +2408,7 @@
         <v>45072</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -2420,7 +2438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -2450,7 +2468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -2481,8 +2499,8 @@
       </c>
       <c r="K45" s="13"/>
     </row>
-    <row r="49" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
@@ -2496,7 +2514,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>56</v>
       </c>
@@ -2510,7 +2528,7 @@
       <c r="J51" s="5"/>
       <c r="K51" s="6"/>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>59</v>
       </c>
@@ -2524,7 +2542,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="6"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>64</v>
       </c>
@@ -2538,7 +2556,7 @@
       <c r="J53" s="5"/>
       <c r="K53" s="6"/>
     </row>
-    <row r="54" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11" t="s">
         <v>67</v>
       </c>
@@ -2568,21 +2586,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5455F7E-3498-453E-982D-C120B5675E13}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
-    <col min="9" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -2618,7 +2636,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -2650,7 +2668,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -2680,7 +2698,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -2710,7 +2728,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -2740,7 +2758,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -2770,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -2800,7 +2818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -2830,7 +2848,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -2860,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -2890,7 +2908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -2920,7 +2938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -2956,7 +2974,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -2988,7 +3006,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -3018,7 +3036,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -3048,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -3078,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -3108,7 +3126,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -3138,7 +3156,7 @@
         <v>44491</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -3168,7 +3186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -3198,7 +3216,7 @@
         <v>44629</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -3228,7 +3246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -3258,7 +3276,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -3288,7 +3306,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -3326,7 +3344,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -3356,7 +3374,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -3386,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -3416,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -3446,7 +3464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -3476,7 +3494,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -3506,7 +3524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -3536,7 +3554,7 @@
         <v>44933</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -3566,7 +3584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -3596,7 +3614,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -3632,7 +3650,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -3664,7 +3682,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -3694,7 +3712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -3724,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -3754,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -3784,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -3814,7 +3832,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -3844,7 +3862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -3874,7 +3892,7 @@
         <v>45072</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -3904,7 +3922,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -3934,7 +3952,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -3970,8 +3988,8 @@
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="49" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
@@ -3990,7 +4008,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>65</v>
       </c>
@@ -4009,7 +4027,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>58</v>
       </c>
@@ -4028,7 +4046,7 @@
       <c r="O52" s="5"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>61</v>
       </c>
@@ -4047,7 +4065,7 @@
       <c r="O53" s="5"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>66</v>
       </c>
@@ -4066,7 +4084,7 @@
       <c r="O54" s="5"/>
       <c r="P54" s="6"/>
     </row>
-    <row r="55" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="11"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -4097,24 +4115,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AD42EA-A0EE-4986-A449-DEBA14E52DE4}">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37" style="15" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="37" style="15" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="37" style="15" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -4126,23 +4143,33 @@
         <v>108</v>
       </c>
       <c r="E1" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="H1" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="I1" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>123</v>
+      </c>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -4161,26 +4188,50 @@
       <c r="F2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="15">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D3" s="15">
         <v>50</v>
       </c>
       <c r="E3" s="15">
+        <v>20</v>
+      </c>
+      <c r="F3" s="15">
+        <v>20</v>
+      </c>
+      <c r="G3" s="15">
+        <v>60</v>
+      </c>
+      <c r="H3" s="15">
         <v>50</v>
       </c>
-      <c r="F3" s="15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I3" s="15">
+        <v>20</v>
+      </c>
+      <c r="J3" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -4197,8 +4248,20 @@
       <c r="F4" s="16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -4215,8 +4278,20 @@
       <c r="F5" s="16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G5" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -4233,8 +4308,20 @@
       <c r="F6" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -4251,8 +4338,20 @@
       <c r="F7" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -4269,8 +4368,20 @@
       <c r="F8" s="25">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G8" s="25">
+        <v>85</v>
+      </c>
+      <c r="H8" s="25">
+        <v>85</v>
+      </c>
+      <c r="I8" s="25">
+        <v>85</v>
+      </c>
+      <c r="J8" s="25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -4287,8 +4398,20 @@
       <c r="F9" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+      <c r="I9" s="16">
+        <v>0</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -4305,8 +4428,20 @@
       <c r="F10" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -4323,8 +4458,20 @@
       <c r="F11" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -4336,23 +4483,33 @@
         <v>62</v>
       </c>
       <c r="E12" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="H12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="I12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -4365,14 +4522,26 @@
       <c r="D13" t="s">
         <v>117</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I13" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -4383,14 +4552,26 @@
       <c r="D14" s="16">
         <v>44</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="16">
         <v>3</v>
       </c>
       <c r="F14" s="16">
+        <v>4</v>
+      </c>
+      <c r="G14" s="31">
+        <v>3</v>
+      </c>
+      <c r="H14" s="16">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I14" s="16">
+        <v>3</v>
+      </c>
+      <c r="J14" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -4401,14 +4582,26 @@
       <c r="D15" s="16">
         <v>0</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="16">
         <v>0</v>
       </c>
       <c r="F15" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G15" s="31">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -4419,14 +4612,26 @@
       <c r="D16" s="16">
         <v>0</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="16">
         <v>0</v>
       </c>
       <c r="F16" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G16" s="31">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -4437,14 +4642,26 @@
       <c r="D17" s="16">
         <v>87</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="16">
         <v>0</v>
       </c>
       <c r="F17" s="16">
+        <v>0</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0</v>
+      </c>
+      <c r="H17" s="16">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I17" s="16">
+        <v>0</v>
+      </c>
+      <c r="J17" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -4455,14 +4672,26 @@
       <c r="D18" s="17">
         <v>44464</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="17">
+        <v>44640</v>
+      </c>
+      <c r="F18" s="17">
+        <v>44811</v>
+      </c>
+      <c r="G18" s="32">
         <v>44256</v>
       </c>
-      <c r="F18" s="17">
+      <c r="H18" s="17">
         <v>44464</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I18" s="17">
+        <v>44640</v>
+      </c>
+      <c r="J18" s="17">
+        <v>44811</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -4473,14 +4702,26 @@
       <c r="D19" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -4491,14 +4732,26 @@
       <c r="D20" s="17">
         <v>44602</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="17">
+        <v>44810</v>
+      </c>
+      <c r="F20" s="17">
+        <v>44862</v>
+      </c>
+      <c r="G20" s="32">
         <v>44409</v>
       </c>
-      <c r="F20" s="17">
+      <c r="H20" s="17">
         <v>44602</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I20" s="17">
+        <v>44810</v>
+      </c>
+      <c r="J20" s="17">
+        <v>44862</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -4509,14 +4762,26 @@
       <c r="D21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="H21" s="16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -4527,14 +4792,26 @@
       <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -4545,14 +4822,26 @@
       <c r="D23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E23" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -4563,26 +4852,36 @@
         <v>117</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G24" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
+      <c r="H24" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -4591,16 +4890,28 @@
         <v>44</v>
       </c>
       <c r="D25" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E25" s="16">
+        <v>4</v>
+      </c>
+      <c r="F25" s="16">
+        <v>4</v>
+      </c>
+      <c r="G25" s="16">
         <v>44</v>
       </c>
-      <c r="F25" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H25" s="16">
+        <v>3</v>
+      </c>
+      <c r="I25" s="16">
+        <v>4</v>
+      </c>
+      <c r="J25" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -4617,8 +4928,20 @@
       <c r="F26" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+      <c r="I26" s="16">
+        <v>0</v>
+      </c>
+      <c r="J26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -4635,8 +4958,20 @@
       <c r="F27" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+      <c r="I27" s="16">
+        <v>0</v>
+      </c>
+      <c r="J27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -4645,16 +4980,28 @@
         <v>87</v>
       </c>
       <c r="D28" s="16">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E28" s="16">
+        <v>0</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0</v>
+      </c>
+      <c r="G28" s="16">
         <v>87</v>
       </c>
-      <c r="F28" s="16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+      <c r="I28" s="16">
+        <v>0</v>
+      </c>
+      <c r="J28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -4666,14 +5013,25 @@
         <v>44640</v>
       </c>
       <c r="E29" s="17">
+        <v>44811</v>
+      </c>
+      <c r="F29" s="17">
+        <v>44863</v>
+      </c>
+      <c r="G29" s="17">
         <v>44464</v>
       </c>
-      <c r="F29" s="17">
+      <c r="H29" s="17">
         <v>44640</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I29" s="17">
+        <v>44811</v>
+      </c>
+      <c r="J29" s="17">
+        <v>44863</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -4685,13 +5043,25 @@
         <v>16</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -4700,16 +5070,28 @@
         <v>44602</v>
       </c>
       <c r="D31" s="17">
-        <v>44895</v>
+        <v>44810</v>
       </c>
       <c r="E31" s="17">
-        <v>44602</v>
+        <v>44862</v>
       </c>
       <c r="F31" s="17">
         <v>44895</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G31" s="17">
+        <v>44602</v>
+      </c>
+      <c r="H31" s="17">
+        <v>44810</v>
+      </c>
+      <c r="I31" s="17">
+        <v>44862</v>
+      </c>
+      <c r="J31" s="17">
+        <v>44895</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -4718,16 +5100,28 @@
         <v>50</v>
       </c>
       <c r="D32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -4738,14 +5132,26 @@
       <c r="D33" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E33" t="s">
-        <v>21</v>
+      <c r="E33" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G33" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -4754,26 +5160,36 @@
         <v>23</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>23</v>
+        <v>120</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
+        <v>120</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>120</v>
+      </c>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -4783,17 +5199,29 @@
       <c r="C35" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="31" t="s">
-        <v>68</v>
+      <c r="D35" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G35" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -4801,17 +5229,29 @@
       <c r="C36" s="16">
         <v>1</v>
       </c>
-      <c r="D36" s="31">
-        <v>3</v>
+      <c r="D36" s="16">
+        <v>4</v>
       </c>
       <c r="E36" s="16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F36" s="31">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G36" s="16">
+        <v>1</v>
+      </c>
+      <c r="H36" s="16">
+        <v>4</v>
+      </c>
+      <c r="I36" s="16">
+        <v>4</v>
+      </c>
+      <c r="J36" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -4819,7 +5259,7 @@
       <c r="C37" s="16">
         <v>0</v>
       </c>
-      <c r="D37" s="31">
+      <c r="D37" s="16">
         <v>0</v>
       </c>
       <c r="E37" s="16">
@@ -4828,8 +5268,20 @@
       <c r="F37" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G37" s="16">
+        <v>0</v>
+      </c>
+      <c r="H37" s="16">
+        <v>0</v>
+      </c>
+      <c r="I37" s="16">
+        <v>0</v>
+      </c>
+      <c r="J37" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -4837,7 +5289,7 @@
       <c r="C38" s="16">
         <v>0</v>
       </c>
-      <c r="D38" s="31">
+      <c r="D38" s="16">
         <v>0</v>
       </c>
       <c r="E38" s="16">
@@ -4846,8 +5298,20 @@
       <c r="F38" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G38" s="16">
+        <v>0</v>
+      </c>
+      <c r="H38" s="16">
+        <v>0</v>
+      </c>
+      <c r="I38" s="16">
+        <v>0</v>
+      </c>
+      <c r="J38" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -4855,17 +5319,29 @@
       <c r="C39" s="16">
         <v>14</v>
       </c>
-      <c r="D39" s="31">
+      <c r="D39" s="16">
         <v>0</v>
       </c>
       <c r="E39" s="16">
+        <v>0</v>
+      </c>
+      <c r="F39" s="31">
+        <v>0</v>
+      </c>
+      <c r="G39" s="16">
         <v>14</v>
       </c>
-      <c r="F39" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="16">
+        <v>0</v>
+      </c>
+      <c r="J39" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -4873,17 +5349,29 @@
       <c r="C40" s="17">
         <v>44640</v>
       </c>
-      <c r="D40" s="32">
-        <v>44986</v>
+      <c r="D40" s="17">
+        <v>44811</v>
       </c>
       <c r="E40" s="17">
-        <v>44640</v>
+        <v>44863</v>
       </c>
       <c r="F40" s="32">
         <v>44986</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G40" s="17">
+        <v>44640</v>
+      </c>
+      <c r="H40" s="17">
+        <v>44811</v>
+      </c>
+      <c r="I40" s="17">
+        <v>44863</v>
+      </c>
+      <c r="J40" s="32">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -4891,18 +5379,29 @@
       <c r="C41" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="31" t="s">
-        <v>16</v>
+      <c r="D41" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G41" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -4911,7 +5410,7 @@
         <v>44895</v>
       </c>
       <c r="D42" s="17">
-        <v>45072</v>
+        <v>44862</v>
       </c>
       <c r="E42" s="17">
         <v>44895</v>
@@ -4919,8 +5418,20 @@
       <c r="F42" s="17">
         <v>45072</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G42" s="17">
+        <v>44895</v>
+      </c>
+      <c r="H42" s="17">
+        <v>44862</v>
+      </c>
+      <c r="I42" s="17">
+        <v>44895</v>
+      </c>
+      <c r="J42" s="17">
+        <v>45072</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -4928,17 +5439,29 @@
       <c r="C43" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="31" t="s">
-        <v>19</v>
+      <c r="D43" s="16" t="s">
+        <v>63</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G43" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -4946,8 +5469,8 @@
       <c r="C44" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D44" s="31" t="s">
-        <v>21</v>
+      <c r="D44" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>53</v>
@@ -4955,8 +5478,20 @@
       <c r="F44" s="31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G44" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I44" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -4964,47 +5499,59 @@
       <c r="C45" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="33" t="s">
-        <v>23</v>
+      <c r="D45" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="F45" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
+      <c r="G45" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="J45" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
-    </row>
-    <row r="49" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+    </row>
+    <row r="49" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="20"/>
-      <c r="E50" s="19"/>
+      <c r="E50" s="20"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
-      <c r="P50" s="3"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="3"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>60</v>
       </c>
@@ -5012,18 +5559,20 @@
       <c r="D51" s="21"/>
       <c r="E51" s="21"/>
       <c r="F51" s="21"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
-      <c r="P51" s="6"/>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="6"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>61</v>
       </c>
@@ -5031,50 +5580,56 @@
       <c r="D52" s="21"/>
       <c r="E52" s="21"/>
       <c r="F52" s="21"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
-      <c r="P52" s="6"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="6"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
       <c r="E53" s="21"/>
       <c r="F53" s="21"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
-      <c r="P53" s="6"/>
-    </row>
-    <row r="54" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="6"/>
+    </row>
+    <row r="54" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
       <c r="K54" s="7"/>
       <c r="L54" s="7"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
-      <c r="P54" s="8"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5096,17 +5651,17 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="7" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" style="15" customWidth="1"/>
-    <col min="9" max="10" width="30.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14" t="s">
         <v>54</v>
@@ -5141,7 +5696,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
@@ -5173,7 +5728,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -5203,7 +5758,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>69</v>
@@ -5233,7 +5788,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -5263,7 +5818,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>72</v>
@@ -5293,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>1</v>
@@ -5323,7 +5878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -5353,7 +5908,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -5383,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -5413,7 +5968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" t="s">
         <v>7</v>
@@ -5443,7 +5998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -5478,7 +6033,7 @@
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -5510,7 +6065,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" t="s">
         <v>74</v>
@@ -5540,7 +6095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -5570,7 +6125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" t="s">
         <v>12</v>
@@ -5600,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" t="s">
         <v>13</v>
@@ -5630,7 +6185,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -5660,7 +6215,7 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" t="s">
         <v>15</v>
@@ -5690,7 +6245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" t="s">
         <v>17</v>
@@ -5720,7 +6275,7 @@
         <v>44614</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" t="s">
         <v>18</v>
@@ -5750,7 +6305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -5780,7 +6335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -5810,7 +6365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>48</v>
       </c>
@@ -5847,7 +6402,7 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" t="s">
         <v>75</v>
@@ -5877,7 +6432,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -5907,7 +6462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" t="s">
         <v>26</v>
@@ -5937,7 +6492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" t="s">
         <v>27</v>
@@ -5967,7 +6522,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" t="s">
         <v>28</v>
@@ -5997,7 +6552,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" t="s">
         <v>29</v>
@@ -6027,7 +6582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -6057,7 +6612,7 @@
         <v>44852</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" t="s">
         <v>31</v>
@@ -6087,7 +6642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" t="s">
         <v>33</v>
@@ -6117,7 +6672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="13" t="s">
         <v>34</v>
@@ -6152,7 +6707,7 @@
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -6184,7 +6739,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" t="s">
         <v>76</v>
@@ -6214,7 +6769,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" t="s">
         <v>37</v>
@@ -6244,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" t="s">
         <v>38</v>
@@ -6274,7 +6829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" t="s">
         <v>39</v>
@@ -6304,7 +6859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" t="s">
         <v>40</v>
@@ -6334,7 +6889,7 @@
         <v>45056</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" t="s">
         <v>41</v>
@@ -6364,7 +6919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" t="s">
         <v>42</v>
@@ -6394,7 +6949,7 @@
         <v>45072</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" t="s">
         <v>43</v>
@@ -6424,7 +6979,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" t="s">
         <v>44</v>
@@ -6454,7 +7009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="13" t="s">
         <v>45</v>
@@ -6489,8 +7044,8 @@
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
     </row>
-    <row r="49" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>51</v>
       </c>
@@ -6508,7 +7063,7 @@
       <c r="N50" s="2"/>
       <c r="O50" s="3"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
@@ -6524,7 +7079,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="6"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
@@ -6540,7 +7095,7 @@
       <c r="N52" s="5"/>
       <c r="O52" s="6"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -6556,7 +7111,7 @@
       <c r="N53" s="5"/>
       <c r="O53" s="6"/>
     </row>
-    <row r="54" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>

</xml_diff>